<commit_message>
update Wed Nov  8 17:42:12 EST 2017
</commit_message>
<xml_diff>
--- a/Source data tables for VISta.xlsx
+++ b/Source data tables for VISta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="7040" tabRatio="500"/>
+    <workbookView xWindow="2860" yWindow="22060" windowWidth="33600" windowHeight="9760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="157">
   <si>
     <t>gnomAD main VCF</t>
   </si>
@@ -182,9 +182,6 @@
     <t>https://storage.googleapis.com/gnomad-public/release/2.0.1/coverage/combined_tars/gnomad.exomes.r2.0.1.coverage.all.tar</t>
   </si>
   <si>
-    <t>Parse into table with one human interval per row and each species sequence is a column</t>
-  </si>
-  <si>
     <t>http://www.sesep.uvsq.fr/03_hypo_mutations.php</t>
   </si>
   <si>
@@ -262,9 +259,6 @@
   </si>
   <si>
     <t>/sc/orga/projects/AILUN/VISta/data/rawdata/repeatmasker/release-April-27-2009/rmsk.txt</t>
-  </si>
-  <si>
-    <t>/sc/orga/projects/AILUN/VISta/data/rawdata/multiz100way/release-multiz100wayrefGene.exonAA.fa</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -424,19 +418,9 @@
     <t>Need to copy paste nine pages or inquire back in the future for an API</t>
   </si>
   <si>
-    <t>AmbryGenetics's AmbryShare</t>
-  </si>
-  <si>
-    <t>https://share.ambrygen.com/login</t>
-  </si>
-  <si>
     <t>/sc/orga/projects/AILUN/soensz01_temp/refGene.201710.with_versions.txt
 /sc/orga/projects/AILUN/soensz01_temp/gbCdnaInfo.201710.txt.gz
 /sc/orga/projects/AILUN/soensz01_temp/refGene.uta_all.unique_aligner</t>
-  </si>
-  <si>
-    <t>Preprocessing to do for maximal data and the minerva location of the script that does it
-(instructions for future updates)</t>
   </si>
   <si>
     <t>Multi-allelic sites if any need to be split into one variant per row
@@ -506,10 +490,6 @@
 UTA database</t>
   </si>
   <si>
-    <t>Use /hpc/users/soensz01/scripts/add_version_to_refGene.pl to add the transcript version (or use simple SQL join).  Add new transcript versions to /sc/orga/projects/AILUN/soensz01_temp/refGene.uta_all.unique_aligner.  Which has the historic versions already present from UTA
-... ADD ADDITIONAL SCRIPTS FOR PROCESSING ...</t>
-  </si>
-  <si>
     <t>Functional assay databases?</t>
   </si>
   <si>
@@ -564,6 +544,22 @@
   <si>
     <t>AA sub matrix
 (grantham / blossum )</t>
+  </si>
+  <si>
+    <t>/sc/orga/projects/AILUN/VISta/data/rawdata/multiz100way/release-multiz100way/refGene.exonAA.fa.gz
+/sc/orga/projects/AILUN/VISta/data/rawdata/multiz100way/release-multiz100way/refGene.exonNuc.fa.gz</t>
+  </si>
+  <si>
+    <t>Preprocessing to do for maximal data and the minerva location of the script that does it
+(instructions for future updates - PLEASE SEE [VISta timeline.xlsx] for updated todos)</t>
+  </si>
+  <si>
+    <t>Parse into table with one human interval per row and each possible species's sequence is a column, if a species is not present in the interval note as NA or null, if all gaps note all gaps
+Is there ever more than one alignment for a single hg19 position? (multi gene/transcript?)</t>
+  </si>
+  <si>
+    <t>Use /hpc/users/soensz01/scripts/add_version_to_refGene.pl to add the transcript version (or use SQL join).  Add new transcript versions to /sc/orga/projects/AILUN/soensz01_temp/refGene.uta_all.unique_aligner.  Which has the historic versions already present from UTA
+... ADD ADDITIONAL SCRIPTS FOR PROCESSING ...</t>
   </si>
 </sst>
 </file>
@@ -748,13 +744,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -765,9 +763,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -834,9 +829,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -864,12 +856,6 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -927,6 +913,24 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -939,28 +943,12 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1237,45 +1225,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="13" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="37.1640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="28.5" style="12" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="37.1640625" style="12" customWidth="1"/>
     <col min="4" max="4" width="124.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="85.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="85" style="13" customWidth="1"/>
-    <col min="7" max="7" width="66.5" style="13" customWidth="1"/>
+    <col min="6" max="6" width="85" style="12" customWidth="1"/>
+    <col min="7" max="7" width="66.5" style="12" customWidth="1"/>
     <col min="8" max="8" width="97.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="67" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="53" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="66" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="64" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="85" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1283,790 +1271,772 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="19" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" s="26"/>
+      <c r="H3" s="17"/>
+    </row>
+    <row r="4" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="59"/>
+      <c r="C4" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="38" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="15" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="15" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" s="15" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="38" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="32" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="59"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="59"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="32" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="59"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="31"/>
+    </row>
+    <row r="20" spans="1:8" s="15" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="59"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" s="15" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="59"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A22" s="59"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="20" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="56" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>149</v>
-      </c>
-      <c r="F3" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="16" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="29" t="s">
+      <c r="F22" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" s="59"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="59"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A25" s="59"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A26" s="59"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="1:8" s="32" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="59"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="28"/>
+    </row>
+    <row r="28" spans="1:8" s="45" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+    </row>
+    <row r="29" spans="1:8" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="38" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="38" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="42" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="F6" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="G6" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" s="43" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="16" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="16" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="G31" s="46"/>
+      <c r="H31" s="36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="19" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" s="50" t="s">
+        <v>156</v>
+      </c>
+      <c r="G32" s="18"/>
+      <c r="H32" s="21"/>
+    </row>
+    <row r="33" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="36"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+    </row>
+    <row r="34" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="19" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="G35" s="18"/>
+      <c r="H35" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="19" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="29"/>
-    </row>
-    <row r="9" spans="1:8" s="16" customFormat="1" ht="112" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="63" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="G36" s="21"/>
+      <c r="H36" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="42" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" s="47" t="s">
-        <v>129</v>
-      </c>
-      <c r="F11" s="47" t="s">
-        <v>129</v>
-      </c>
-      <c r="G11" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="H11" s="43" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+    </row>
+    <row r="37" spans="1:8" s="19" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="34" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="33"/>
-    </row>
-    <row r="15" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" t="s">
-        <v>120</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="E37" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="37"/>
-    </row>
-    <row r="16" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="17" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="16" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="62"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18" s="11" t="s">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="62"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A20" s="62"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="F20" s="46" t="s">
+      <c r="B39" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="33"/>
-    </row>
-    <row r="21" spans="1:8" s="16" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="62"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F21" s="11" t="s">
+      <c r="C39" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="61"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G40" s="10"/>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" s="16" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="62"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" s="16" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A23" s="62"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:8" s="20" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A24" s="62"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-    </row>
-    <row r="25" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="62"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="1:8" s="16" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A26" s="62"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:8" s="16" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A27" s="62"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="1:8" s="34" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="62"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="E28" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="30"/>
-    </row>
-    <row r="29" spans="1:8" s="49" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="48"/>
-      <c r="F29" s="47" t="s">
-        <v>129</v>
-      </c>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-    </row>
-    <row r="30" spans="1:8" s="16" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="63" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="42" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="63"/>
-      <c r="C31" s="63" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="47" t="s">
-        <v>129</v>
-      </c>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="42" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="G32" s="50"/>
-      <c r="H32" s="40" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="20" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="63" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="23" t="s">
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="E33" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="F33" s="54" t="s">
-        <v>141</v>
-      </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-    </row>
-    <row r="35" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" s="19"/>
-      <c r="H36" s="22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="20" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G37" s="22"/>
-      <c r="H37" s="19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="20" customFormat="1" ht="144" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="51" t="s">
-        <v>142</v>
-      </c>
-      <c r="B40" s="58" t="s">
-        <v>144</v>
-      </c>
-      <c r="C40" s="58" t="s">
-        <v>145</v>
-      </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="59"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G41" s="11"/>
-      <c r="H41" s="12"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B42" s="59"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="6"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="60" t="s">
-        <v>146</v>
-      </c>
-      <c r="B43" s="59"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="6"/>
+      <c r="A43" s="63"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
+      <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="61"/>
-      <c r="B44" s="59"/>
-      <c r="C44" s="59"/>
-      <c r="H44" s="13"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="61"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="59"/>
-      <c r="H45" s="13"/>
+      <c r="A44" s="63"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
+      <c r="H44" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="C39:C44"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C30:C31"/>
     <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B29"/>
+    <mergeCell ref="B10:B28"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C10:C29"/>
+    <mergeCell ref="C10:C28"/>
     <mergeCell ref="C6:C9"/>
-    <mergeCell ref="B40:B45"/>
-    <mergeCell ref="C40:C45"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A17:A28"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C31:C32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update Mon Nov 13 17:34:49 EST 2017
</commit_message>
<xml_diff>
--- a/Source data tables for VISta.xlsx
+++ b/Source data tables for VISta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="22060" windowWidth="33600" windowHeight="9760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="158">
   <si>
     <t>gnomAD main VCF</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>http://geneticmedicine.weill.cornell.edu/genome.html</t>
-  </si>
-  <si>
-    <t>db2.resilience, db2.newborn, manual additions</t>
   </si>
   <si>
     <t>ClinVar</t>
@@ -418,11 +415,6 @@
     <t>Need to copy paste nine pages or inquire back in the future for an API</t>
   </si>
   <si>
-    <t>/sc/orga/projects/AILUN/soensz01_temp/refGene.201710.with_versions.txt
-/sc/orga/projects/AILUN/soensz01_temp/gbCdnaInfo.201710.txt.gz
-/sc/orga/projects/AILUN/soensz01_temp/refGene.uta_all.unique_aligner</t>
-  </si>
-  <si>
     <t>Multi-allelic sites if any need to be split into one variant per row
 Left normalize and generate vkey
 What % of sites are covered &gt;20x on average?  Remove sites below or remove individuals below and recalc AF?
@@ -511,10 +503,6 @@
     <t>Gene-phenotype information table</t>
   </si>
   <si>
-    <t>I started merging some files on this, needs a lot more work:
-/sc/orga/projects/AILUN/soensz01_temp/db2.gene.tab</t>
-  </si>
-  <si>
     <t>NA - manually curated</t>
   </si>
   <si>
@@ -550,16 +538,35 @@
 /sc/orga/projects/AILUN/VISta/data/rawdata/multiz100way/release-multiz100way/refGene.exonNuc.fa.gz</t>
   </si>
   <si>
-    <t>Preprocessing to do for maximal data and the minerva location of the script that does it
-(instructions for future updates - PLEASE SEE [VISta timeline.xlsx] for updated todos)</t>
-  </si>
-  <si>
     <t>Parse into table with one human interval per row and each possible species's sequence is a column, if a species is not present in the interval note as NA or null, if all gaps note all gaps
 Is there ever more than one alignment for a single hg19 position? (multi gene/transcript?)</t>
   </si>
   <si>
-    <t>Use /hpc/users/soensz01/scripts/add_version_to_refGene.pl to add the transcript version (or use SQL join).  Add new transcript versions to /sc/orga/projects/AILUN/soensz01_temp/refGene.uta_all.unique_aligner.  Which has the historic versions already present from UTA
-... ADD ADDITIONAL SCRIPTS FOR PROCESSING ...</t>
+    <t>I started merging some files on this, but we are now expecting the gene curation process to provide this info:
+/sc/orga/projects/AILUN/soensz01_temp/db2.gene.tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Instructions for future updates
+(slowly removing todo's and replacing with update instructions)
+PLEASE SEE [VISta timeline.xlsx] for updated todos</t>
+  </si>
+  <si>
+    <t>Use /hpc/users/soensz01/scripts/add_version_to_refGene.pl to add the transcript version (or use SQL join).
+Merge new refGene transcript alignments with /hpc/users/soensz01/AILUN/soensz01_temp/refGene.uta_all.unique_aligner.refGene_supplemented.no_slashes_in_nms.dups_resolved (which has the historic versions already present from UTA)
+Run resolve_non-unique_alignments_in_a_refGene_table.pl to remove any transcript.versions with multiple alignments</t>
+  </si>
+  <si>
+    <t>/sc/orga/projects/AILUN/soensz01_temp/refGene.201710.with_versions.txt
+/sc/orga/projects/AILUN/soensz01_temp/gbCdnaInfo.201710.txt.gz
+/sc/orga/projects/AILUN/soensz01_temp/refGene.uta_all.unique_aligner
+UTA database work should not need to be repeated</t>
+  </si>
+  <si>
+    <t>gene curation project</t>
+  </si>
+  <si>
+    <t>/hpc/users/soensz01/AILUN/soensz01_temp/refGene.uta_all.unique_aligner.refGene_201710_supplemented.dups_resolved</t>
   </si>
 </sst>
 </file>
@@ -752,7 +759,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -802,9 +809,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -829,9 +833,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -901,46 +902,49 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1227,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="62" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1245,702 +1249,706 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="49" t="s">
-        <v>151</v>
-      </c>
-      <c r="C1" s="55" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="85" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="H3" s="57"/>
+    </row>
+    <row r="4" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="55"/>
+      <c r="C4" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="19" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+    </row>
+    <row r="5" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="58" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="F3" s="54" t="s">
-        <v>144</v>
-      </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="G5" s="11"/>
+      <c r="H5" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="36" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="27" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="38" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="57" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="39" t="s">
-        <v>86</v>
+      <c r="H6" s="37" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="15" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G7" s="10"/>
-      <c r="H7" s="27" t="s">
-        <v>57</v>
+      <c r="H7" s="25" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="15" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="35" t="s">
-        <v>122</v>
-      </c>
       <c r="E8" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G8" s="10"/>
-      <c r="H8" s="27"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" s="15" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
       <c r="D9" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="E10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="38" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="39" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="22" t="s">
+      <c r="F12" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="20"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
+        <v>106</v>
+      </c>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="29"/>
+    </row>
+    <row r="15" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="27" t="s">
+      <c r="F16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="32" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="20"/>
-    </row>
-    <row r="16" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
     <row r="17" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="59"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="59"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
       <c r="D18" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G18" s="10"/>
-      <c r="H18" s="27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="32" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A19" s="59"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="31"/>
+      <c r="H18" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="56"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="26"/>
+      <c r="H19" s="29"/>
     </row>
     <row r="20" spans="1:8" s="15" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="59"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" s="15" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="59"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
       <c r="D21" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>115</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A22" s="59"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
+      <c r="A22" s="56"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
       <c r="D22" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:8" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A23" s="59"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="24" t="s">
+    <row r="23" spans="1:8" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" s="56"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+    </row>
+    <row r="24" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="56"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-    </row>
-    <row r="24" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="59"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="F24" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A25" s="59"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
       <c r="D25" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="F25" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>93</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A26" s="59"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
       <c r="D26" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>97</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:8" s="32" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="59"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="28"/>
-    </row>
-    <row r="28" spans="1:8" s="45" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="44"/>
-      <c r="F28" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
+    <row r="27" spans="1:8" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="56"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="26"/>
+    </row>
+    <row r="28" spans="1:8" s="43" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="42"/>
+      <c r="F28" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
     </row>
     <row r="29" spans="1:8" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="D29" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="56"/>
+      <c r="C30" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="56"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="G31" s="44"/>
+      <c r="H31" s="34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="36" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="34"/>
+      <c r="C32" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="G32" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="H32" s="34"/>
+    </row>
+    <row r="33" spans="1:8" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="34"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+    </row>
+    <row r="34" spans="1:8" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="38" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" s="36" t="s">
+    <row r="35" spans="1:8" s="18" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="38" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="46"/>
-      <c r="H31" s="36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="19" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32" s="50" t="s">
-        <v>156</v>
-      </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="21"/>
-    </row>
-    <row r="33" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-    </row>
-    <row r="34" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36" t="s">
+      <c r="E35" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="G35" s="17"/>
+      <c r="H35" s="20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="19" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A35" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="G35" s="18"/>
-      <c r="H35" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="19" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21" t="s">
+    <row r="36" spans="1:8" s="18" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="G36" s="20"/>
+      <c r="H36" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="18" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+      <c r="A37" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="G36" s="21"/>
-      <c r="H36" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="19" customFormat="1" ht="144" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="18" t="s">
-        <v>12</v>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="17" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1954,14 +1962,14 @@
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="60" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" s="60" t="s">
-        <v>139</v>
+      <c r="C39" s="51" t="s">
+        <v>137</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -1971,28 +1979,28 @@
     </row>
     <row r="40" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="61"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="E40" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="11"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B41" s="61"/>
-      <c r="C41" s="61"/>
+        <v>135</v>
+      </c>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="5"/>
@@ -2000,11 +2008,11 @@
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="62" t="s">
-        <v>140</v>
-      </c>
-      <c r="B42" s="61"/>
-      <c r="C42" s="61"/>
+      <c r="A42" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="5"/>
@@ -2012,19 +2020,24 @@
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="63"/>
-      <c r="B43" s="61"/>
-      <c r="C43" s="61"/>
+      <c r="A43" s="54"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="63"/>
-      <c r="B44" s="61"/>
-      <c r="C44" s="61"/>
+      <c r="A44" s="54"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="52"/>
       <c r="H44" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B28"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C10:C28"/>
+    <mergeCell ref="C6:C9"/>
     <mergeCell ref="B39:B44"/>
     <mergeCell ref="C39:C44"/>
     <mergeCell ref="A42:A44"/>
@@ -2032,11 +2045,6 @@
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B28"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C10:C28"/>
-    <mergeCell ref="C6:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update Mon Nov 27 18:05:11 EST 2017
</commit_message>
<xml_diff>
--- a/Source data tables for VISta.xlsx
+++ b/Source data tables for VISta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="163">
   <si>
     <t>gnomAD main VCF</t>
   </si>
@@ -207,9 +207,6 @@
     <t>(chr, pos, ref, alt, mean_Depth, RA, AA, NR, NA)</t>
   </si>
   <si>
-    <t>TBD will integrate template and the path from xml</t>
-  </si>
-  <si>
     <t>(Nucleotide_change, Classification)</t>
   </si>
   <si>
@@ -292,18 +289,6 @@
   </si>
   <si>
     <t>/hpc/users/soensz01/AILUN/soensz01_temp/PAH_functional_studies.txt</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(chr, pos, ref, alt) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>also genotype counts and MAF for each ethnicity</t>
-    </r>
   </si>
   <si>
     <t>(pmid, acc_num) adding (chr, pos, ref, alt) to generate vKey.</t>
@@ -552,11 +537,6 @@
 PLEASE SEE [VISta timeline.xlsx] for updated todos</t>
   </si>
   <si>
-    <t>Use /hpc/users/soensz01/scripts/add_version_to_refGene.pl to add the transcript version (or use SQL join).
-Merge new refGene transcript alignments with /hpc/users/soensz01/AILUN/soensz01_temp/refGene.uta_all.unique_aligner.refGene_supplemented.no_slashes_in_nms.dups_resolved (which has the historic versions already present from UTA)
-Run resolve_non-unique_alignments_in_a_refGene_table.pl to remove any transcript.versions with multiple alignments</t>
-  </si>
-  <si>
     <t>/sc/orga/projects/AILUN/soensz01_temp/refGene.201710.with_versions.txt
 /sc/orga/projects/AILUN/soensz01_temp/gbCdnaInfo.201710.txt.gz
 /sc/orga/projects/AILUN/soensz01_temp/refGene.uta_all.unique_aligner
@@ -567,13 +547,43 @@
   </si>
   <si>
     <t>/hpc/users/soensz01/AILUN/soensz01_temp/refGene.uta_all.unique_aligner.refGene_201710_supplemented.dups_resolved</t>
+  </si>
+  <si>
+    <t>Use /add_version_to_refGene.pl to add the transcript version (or use SQL join).
+Overwrite and add new refGene transcript alignments to /refGene.uta_all.unique_aligner.refGene_supplemented.no_slashes_in_nms.dups_resolved (which has the historic versions already present from UTA)
+Run /resolve_non-unique_alignments_in_a_refGene_table.pl to remove any transcript.versions with multiple alignments
+Remove alignments to chromosome scaffolds (chroms with an "_")</t>
+  </si>
+  <si>
+    <t>chr, pos, ref, alt and (AC, AN, AF, genotypes counts for homo, hetero, hemiz) for total and each subpop</t>
+  </si>
+  <si>
+    <t>/sc/orga/projects/AILUN/VISta/data/output_parsed/HGVD/HGVD_201602_v1.csv</t>
+  </si>
+  <si>
+    <t>/sc/orga/projects/AILUN/VISta/data/output_parsed/UK10K/UK10K_COHORT.20160215.sites.csv</t>
+  </si>
+  <si>
+    <t>/sc/orga/projects/AILUN/VISta/data/output_parsed/ClinVar/ClinVar_201710_v8.tsv</t>
+  </si>
+  <si>
+    <t>see multiple table design in: clinvar_v7_10k_with_db2_formats
+(ask Zach)</t>
+  </si>
+  <si>
+    <t>Minerva location of processed minimal data
+(table or multi-table form)
+(should be identical to what is then uploaded into db2)</t>
+  </si>
+  <si>
+    <t>db2 database and table names</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -603,10 +613,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri (Body)"/>
     </font>
     <font>
       <sz val="12"/>
@@ -751,208 +757,215 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1229,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="62" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="56" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1245,29 +1258,30 @@
     <col min="6" max="6" width="85" style="12" customWidth="1"/>
     <col min="7" max="7" width="66.5" style="12" customWidth="1"/>
     <col min="8" max="8" width="97.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="3"/>
+    <col min="9" max="10" width="68" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" s="49" t="s">
+      <c r="E1" s="18" t="s">
         <v>145</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>147</v>
       </c>
       <c r="F1" s="46"/>
       <c r="G1" s="46"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="85" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="85" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1278,50 +1292,58 @@
         <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="E3" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="54" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" s="59" t="s">
-        <v>152</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" s="61" t="s">
+      <c r="G3" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="57"/>
-    </row>
-    <row r="4" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="51"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+    </row>
+    <row r="4" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="55"/>
+      <c r="B4" s="62"/>
       <c r="C4" s="29" t="s">
         <v>31</v>
       </c>
@@ -1329,15 +1351,17 @@
         <v>15</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" s="29"/>
       <c r="G4" s="29"/>
       <c r="H4" s="29" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+    </row>
+    <row r="5" spans="1:10" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>42</v>
       </c>
@@ -1351,86 +1375,98 @@
         <v>47</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="36" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:10" s="36" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="56" t="s">
+      <c r="B6" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="61" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="35" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="15" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+    </row>
+    <row r="7" spans="1:10" s="15" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A7" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G7" s="10"/>
+        <v>114</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>157</v>
+      </c>
       <c r="H7" s="25" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="15" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:10" s="15" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A8" s="56" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="33" t="s">
-        <v>120</v>
-      </c>
       <c r="E8" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G8" s="10"/>
+        <v>114</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>158</v>
+      </c>
       <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="1:8" s="15" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:10" s="15" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="14" t="s">
         <v>5</v>
       </c>
@@ -1438,340 +1474,382 @@
         <v>41</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:10" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="56" t="s">
+      <c r="B10" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="61" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="G10" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H10" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+    </row>
+    <row r="12" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="E11" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="H11" s="37" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="21" t="s">
+      <c r="F12" s="17" t="s">
         <v>126</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>128</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="19"/>
-    </row>
-    <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
+        <v>104</v>
+      </c>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:10" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
+        <v>103</v>
+      </c>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
       <c r="D14" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
       <c r="H14" s="29"/>
-    </row>
-    <row r="15" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+    </row>
+    <row r="15" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
+        <v>96</v>
+      </c>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
       <c r="H15" s="19"/>
-    </row>
-    <row r="16" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="56" t="s">
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="8" t="s">
         <v>52</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="56"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
+        <v>58</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="61"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="56"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="61"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
       <c r="D18" s="8" t="s">
         <v>53</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A19" s="56"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
+        <v>85</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="61"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="39" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F19" s="40" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G19" s="26"/>
       <c r="H19" s="29"/>
-    </row>
-    <row r="20" spans="1:8" s="15" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="56"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" s="15" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
-    </row>
-    <row r="21" spans="1:8" s="15" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="56"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:10" s="15" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="61"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E21" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>114</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A22" s="56"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="56"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:10" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A22" s="61"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="1:8" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A23" s="56"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="1:10" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" s="61"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="23" t="s">
-        <v>83</v>
-      </c>
       <c r="F23" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
-    </row>
-    <row r="24" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="56"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="61"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
       <c r="D24" s="8" t="s">
         <v>48</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
-    </row>
-    <row r="25" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A25" s="56"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:10" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A25" s="61"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
       <c r="D25" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="1:8" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A26" s="56"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="56"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="1:10" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A26" s="61"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
       <c r="D26" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E26" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>96</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
-    </row>
-    <row r="27" spans="1:8" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="56"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="1:10" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="61"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
       <c r="H27" s="26"/>
-    </row>
-    <row r="28" spans="1:8" s="43" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+    </row>
+    <row r="28" spans="1:10" s="43" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="42" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="42"/>
       <c r="F28" s="41" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
-    </row>
-    <row r="29" spans="1:8" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+    </row>
+    <row r="29" spans="1:10" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="61" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="10" t="s">
@@ -1781,95 +1859,105 @@
         <v>22</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:10" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="55" t="s">
+      <c r="B30" s="61"/>
+      <c r="C30" s="62" t="s">
         <v>36</v>
       </c>
       <c r="D30" s="35" t="s">
         <v>23</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G30" s="34"/>
       <c r="H30" s="34" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+    </row>
+    <row r="31" spans="1:10" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="55"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="62"/>
       <c r="D31" s="35" t="s">
         <v>29</v>
       </c>
       <c r="E31" s="44"/>
       <c r="F31" s="44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G31" s="44"/>
       <c r="H31" s="34" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="36" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="I31" s="35"/>
+      <c r="J31" s="35"/>
+    </row>
+    <row r="32" spans="1:10" s="36" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="34" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="34"/>
-      <c r="C32" s="55" t="s">
+      <c r="C32" s="62" t="s">
         <v>34</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E32" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="F32" s="44" t="s">
+      <c r="G32" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="G32" s="44" t="s">
-        <v>157</v>
-      </c>
       <c r="H32" s="34"/>
-    </row>
-    <row r="33" spans="1:8" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+    </row>
+    <row r="33" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="34" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="34"/>
-      <c r="C33" s="55"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="35" t="s">
         <v>20</v>
       </c>
       <c r="E33" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
-    </row>
-    <row r="34" spans="1:8" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+    </row>
+    <row r="34" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="34" t="s">
         <v>18</v>
       </c>
@@ -1881,15 +1969,17 @@
         <v>17</v>
       </c>
       <c r="E34" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="18" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+    </row>
+    <row r="35" spans="1:10" s="18" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
         <v>21</v>
       </c>
@@ -1901,19 +1991,21 @@
         <v>26</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G35" s="17"/>
       <c r="H35" s="20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="18" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+    </row>
+    <row r="36" spans="1:10" s="18" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="20" t="s">
@@ -1926,21 +2018,23 @@
         <v>11</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" s="18" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+    </row>
+    <row r="37" spans="1:10" s="18" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
         <v>46</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
       <c r="D37" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E37" s="17" t="s">
         <v>11</v>
@@ -1950,8 +2044,10 @@
       <c r="H37" s="17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1960,75 +2056,85 @@
       <c r="F38" s="5"/>
       <c r="G38" s="6"/>
       <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="B39" s="51" t="s">
-        <v>136</v>
-      </c>
-      <c r="C39" s="51" t="s">
-        <v>137</v>
+      <c r="C39" s="57" t="s">
+        <v>135</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="5"/>
       <c r="G39" s="6"/>
       <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="52"/>
-      <c r="C40" s="52"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="58"/>
       <c r="D40" s="11" t="s">
         <v>50</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="11"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B41" s="52"/>
-      <c r="C41" s="52"/>
+        <v>133</v>
+      </c>
+      <c r="B41" s="58"/>
+      <c r="C41" s="58"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="5"/>
       <c r="G41" s="6"/>
       <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="53" t="s">
-        <v>138</v>
-      </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="52"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="59" t="s">
+        <v>136</v>
+      </c>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="5"/>
       <c r="G42" s="6"/>
       <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="54"/>
-      <c r="B43" s="52"/>
-      <c r="C43" s="52"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="60"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="58"/>
       <c r="H43" s="12"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="54"/>
-      <c r="B44" s="52"/>
-      <c r="C44" s="52"/>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="60"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="58"/>
       <c r="H44" s="12"/>
     </row>
   </sheetData>

</xml_diff>